<commit_message>
P5 updates and G7 curve
</commit_message>
<xml_diff>
--- a/data/LowFluoCurveF199_PlateCounts_20231018.xlsx
+++ b/data/LowFluoCurveF199_PlateCounts_20231018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ameliafoley/Desktop/R/encapsulation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D8A1296-9D58-5844-A996-9F9DFA9A7052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C924EEF1-9805-F24D-9F8C-4EBDF4CC25DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16060" xr2:uid="{3E1D5A78-585C-A648-9F2B-B60745060C1D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="6">
   <si>
     <t>sample</t>
   </si>
@@ -89,8 +89,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC830A15-F38A-2E4A-AC10-190FF65B093A}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -432,151 +433,231 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="D2">
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="D3">
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="D4">
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="D5">
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>100000</v>
+      </c>
+      <c r="D6">
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>100000</v>
+      </c>
+      <c r="D7">
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
+      </c>
+      <c r="C8" s="1">
+        <v>100000</v>
+      </c>
+      <c r="D8">
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
+      </c>
+      <c r="C9" s="1">
+        <v>100000</v>
+      </c>
+      <c r="D9">
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
+      </c>
+      <c r="C10" s="1">
+        <v>100000</v>
+      </c>
+      <c r="D10">
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
+      </c>
+      <c r="C11" s="1">
+        <v>100000</v>
+      </c>
+      <c r="D11">
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
+      </c>
+      <c r="C12" s="1">
+        <v>100000</v>
+      </c>
+      <c r="D12">
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
+      </c>
+      <c r="C13" s="1">
+        <v>100000</v>
+      </c>
+      <c r="D13">
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>0.05</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
+      </c>
+      <c r="C14" s="1">
+        <v>10000</v>
+      </c>
+      <c r="D14">
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>0.05</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
+      </c>
+      <c r="C15" s="1">
+        <v>10000</v>
+      </c>
+      <c r="D15">
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>2.5000000000000001E-2</v>
+        <v>0.01</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" s="1">
+        <v>10000</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>2.5000000000000001E-2</v>
+        <v>0.01</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>0.01</v>
-      </c>
-      <c r="B18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>0.01</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
+      <c r="C17" s="1">
+        <v>10000</v>
+      </c>
+      <c r="D17">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D19">
-    <sortCondition descending="1" ref="A2:A19"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D17">
+    <sortCondition descending="1" ref="A2:A17"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>